<commit_message>
day31 - 1eetcode weekly contest
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\NeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E733D02D-6500-4401-B543-DA0EB66F79B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B16D6-5E7F-4C15-8D98-03DDBABBCE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Other Notes" sheetId="2" r:id="rId2"/>
+    <sheet name="leetcode contest note" sheetId="3" r:id="rId2"/>
+    <sheet name="Other Notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="205">
   <si>
     <t>NeetCode - Blind 75</t>
   </si>
@@ -632,13 +633,34 @@
   </si>
   <si>
     <t>backtracking to compute every substring (using ptr and list slices), only proceed when current substring of current partition is palin</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>numpy array is much faster than list, for high performance requirement on numbers, use numpy array over list</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>participant</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,6 +672,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -690,20 +719,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -990,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -1981,6 +2014,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5D96A-E969-4996-897E-90E2435ADE82}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44941</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2">
+        <v>8579</v>
+      </c>
+      <c r="E2">
+        <v>22199</v>
+      </c>
+      <c r="F2" s="6">
+        <f>D2/E2</f>
+        <v>0.38645884949772513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50CDE21C-70B8-4212-8C19-0C4794CBEC94}">
   <dimension ref="A1:P6"/>
   <sheetViews>

</xml_diff>

<commit_message>
day37 - 1eetcode weekly contest
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\NeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48851EFA-5A18-4448-9FDD-F4E8F4AF0CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CAB4CA-930A-405A-9AD4-E46F1F6DB05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="245">
   <si>
     <t>NeetCode - Blind 75</t>
   </si>
@@ -771,6 +771,9 @@
   </si>
   <si>
     <t>like 417, use 2 sets: cap &amp; uncap, run dfs on all border "O", then for all (r,c)in cap, turn to X</t>
+  </si>
+  <si>
+    <t>practise bitwise operation questions</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5D96A-E969-4996-897E-90E2435ADE82}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,6 +2368,27 @@
       <c r="F2" s="6">
         <f>D2/E2</f>
         <v>0.38645884949772513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>44948</v>
+      </c>
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3">
+        <v>8243</v>
+      </c>
+      <c r="E3">
+        <v>16012</v>
+      </c>
+      <c r="F3" s="6">
+        <f>D3/E3</f>
+        <v>0.51480139895078691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day43 - leetcode weekly contest
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\NeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761AB651-C5D3-49FA-8F81-1733E9370014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D19D8B-9EB7-414C-A8BA-8CC863530420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="271">
   <si>
     <t>Array &amp; Hashing</t>
   </si>
@@ -849,6 +849,9 @@
   </si>
   <si>
     <t>compute currMax of each house backwards, use dict to store index: currMax; currMax = max(arr[i] + currMax[i+1], currMax[i])</t>
+  </si>
+  <si>
+    <t>search on Q2 (Count Collisions of Monkeys on a Polygon) later</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+    <sheetView topLeftCell="A98" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -2517,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5D96A-E969-4996-897E-90E2435ADE82}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,6 +2593,27 @@
       <c r="F3" s="6">
         <f>D3/E3</f>
         <v>0.51480139895078691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44953</v>
+      </c>
+      <c r="C4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4">
+        <v>9590</v>
+      </c>
+      <c r="E4">
+        <v>21232</v>
+      </c>
+      <c r="F4" s="6">
+        <f>D4/E4</f>
+        <v>0.45167671439336848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to python day64
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jitianliang/Desktop/GithubRepos/NeetCodePractice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EE99A0-FD4E-8D4A-AA00-436E52362276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAD86CA-4EA0-F842-917D-92399747F8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="-120" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="322">
   <si>
     <t>Array &amp; Hashing</t>
   </si>
@@ -999,6 +999,12 @@
   </si>
   <si>
     <t>use a dummy node (cur = dummy), while cur.next: do the check, return dummy.next</t>
+  </si>
+  <si>
+    <t>75. Sort Colors</t>
+  </si>
+  <si>
+    <t>bucket sort (use a bucket of size n (#of distinct values); 1 pass - 2 ptrs + partition</t>
   </si>
 </sst>
 </file>
@@ -1366,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1578,264 +1584,264 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>6</v>
+        <v>320</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>297</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>298</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>309</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
@@ -1846,1084 +1852,1095 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>312</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>313</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
         <v>315</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>138</v>
+        <v>308</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>139</v>
+        <v>307</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B61" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B64" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="B66" t="s">
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>317</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B68" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>188</v>
+        <v>47</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>189</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>204</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B73" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B76" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
-      </c>
-      <c r="C77" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B81" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C82" t="s">
-        <v>164</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B83" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84" t="s">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B85" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>167</v>
+        <v>64</v>
       </c>
       <c r="B86" t="s">
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>67</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B88" t="s">
         <v>60</v>
       </c>
       <c r="C88" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="B89" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C89" t="s">
-        <v>208</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B90" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B91" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B92" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B94" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B95" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
         <v>79</v>
       </c>
-      <c r="D95">
+      <c r="D96">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B96" t="s">
-        <v>7</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B98" t="s">
-        <v>3</v>
-      </c>
-      <c r="C98" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B100" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
       </c>
       <c r="C101" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
       </c>
       <c r="C102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B103" t="s">
-        <v>7</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B104" t="s">
-        <v>7</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B106" t="s">
-        <v>7</v>
-      </c>
-      <c r="C106" t="s">
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B107" t="s">
-        <v>7</v>
-      </c>
-      <c r="C107" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B108" t="s">
         <v>7</v>
       </c>
       <c r="C108" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
       </c>
       <c r="C109" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B110" t="s">
         <v>7</v>
       </c>
       <c r="C110" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B111" t="s">
         <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B112" t="s">
         <v>7</v>
       </c>
       <c r="C112" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B114" t="s">
-        <v>3</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="B115" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B116" t="s">
-        <v>7</v>
-      </c>
-      <c r="C116" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B118" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="B119" t="s">
         <v>60</v>
       </c>
       <c r="C119" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C120" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="B121" t="s">
         <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B122" t="s">
         <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="B123" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B124" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C124" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B125" t="s">
         <v>7</v>
       </c>
       <c r="C125" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
       </c>
       <c r="C127" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B128" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B128" t="s">
-        <v>3</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="B129" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B130" t="s">
-        <v>60</v>
-      </c>
-      <c r="C130" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B131" t="s">
         <v>60</v>
       </c>
       <c r="C131" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B132" t="s">
         <v>60</v>
       </c>
       <c r="C132" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B133" t="s">
+        <v>60</v>
+      </c>
+      <c r="C133" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B133" t="s">
-        <v>7</v>
-      </c>
-      <c r="C133" t="s">
+      <c r="B134" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B135" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B136" t="s">
-        <v>3</v>
-      </c>
-      <c r="C136" t="s">
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B137" t="s">
-        <v>3</v>
-      </c>
-      <c r="C137" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C138" t="s">
-        <v>154</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>257</v>
+        <v>153</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
       </c>
       <c r="C139" t="s">
-        <v>258</v>
+        <v>154</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B140" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B140" t="s">
-        <v>3</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="B141" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B142" t="s">
-        <v>3</v>
-      </c>
-      <c r="C142" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B143" t="s">
         <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B144" t="s">
-        <v>7</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="B145" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>60</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C147" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B148" t="s">
-        <v>60</v>
-      </c>
-      <c r="C148" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C149" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B150" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B150" t="s">
-        <v>3</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="B151" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" t="s">
         <v>290</v>
       </c>
     </row>

</xml_diff>